<commit_message>
First complete version of atmosphere and ocean biogeochemistry files
</commit_message>
<xml_diff>
--- a/cmip6/models/noresm2-lm/cmip6_ncc_noresm2-lm_ocnbgchem.xlsx
+++ b/cmip6/models/noresm2-lm/cmip6_ncc_noresm2-lm_ocnbgchem.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jetj/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE28CA5-FF8F-D24C-B9A4-0823D03E88F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="4620" yWindow="760" windowWidth="24140" windowHeight="12000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,12 @@
     <sheet name="1. Key Properties" sheetId="3" r:id="rId3"/>
     <sheet name="2. Tracers" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="434">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -1295,13 +1301,37 @@
   </si>
   <si>
     <t>Diagnostic)</t>
+  </si>
+  <si>
+    <t>iHamocc</t>
+  </si>
+  <si>
+    <t>he oceanic carbon cycle component has gone through numerous updates that include, amongst others, improved process representations, increased interactions with the atmosphere, and additional new tracers. Oceanic dimethyl sulfide (DMS) is now prognostically simulated and its fluxes are directly coupled with the atmospheric component, leading to a direct feedback to the climate. Atmospheric nitrogen deposition and additional riverine inputs of other biogeochemical tracers have recently been included in the model. The implementation of new tracers such as “preformed” and “natural” tracers enables a separation of physical from biogeochemical drivers as well as of internal from external forcings and hence a better diagnostic of the simulated biogeochemical variability. Carbon isotope tracers have been implemented and will be relevant for studying long-term past climate changes. </t>
+  </si>
+  <si>
+    <t>All fixed</t>
+  </si>
+  <si>
+    <t>pH, CO3, OmegaC</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Wanninkhof (2014)</t>
+  </si>
+  <si>
+    <t>To improve the large scale mean state surface and interior and upper ocean seasonal cycle.</t>
+  </si>
+  <si>
+    <t>air-sea CO2 fluxes, surface primary productivity, DMS fluxes, export production</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1402,6 +1432,12 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF464646"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1447,7 +1483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1491,17 +1527,26 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1543,7 +1588,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1575,9 +1620,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1609,6 +1672,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1784,24 +1865,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="180.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="35.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="180.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="33" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1809,7 +1890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1817,7 +1898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1825,7 +1906,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1833,7 +1914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1841,12 +1922,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1854,7 +1935,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1862,7 +1943,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1870,7 +1951,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -1878,13 +1959,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
@@ -1892,54 +1973,54 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1"/>
-    <hyperlink ref="B12" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="80.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="80.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="9"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>27</v>
       </c>
@@ -1947,27 +2028,27 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="9"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>27</v>
       </c>
@@ -1975,42 +2056,44 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Author,Contributor,Principal Investigator,Point of Contact,Sponsor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Top Level,Key Properties,Tracers"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1"/>
-    <hyperlink ref="A13" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A13" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD235"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AD235"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" customHeight="1">
+    <row r="1" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>33</v>
       </c>
@@ -2018,12 +2101,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" customHeight="1">
+    <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
@@ -2031,7 +2114,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" customHeight="1">
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>38</v>
       </c>
@@ -2042,12 +2125,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1">
+    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="24" customHeight="1">
+    <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>42</v>
       </c>
@@ -2055,7 +2138,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24" customHeight="1">
+    <row r="9" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>38</v>
       </c>
@@ -2066,15 +2149,17 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24" customHeight="1">
+    <row r="10" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="24" customHeight="1">
-      <c r="B11" s="11"/>
-    </row>
-    <row r="13" spans="1:3" ht="24" customHeight="1">
+    <row r="11" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="11" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>47</v>
       </c>
@@ -2082,7 +2167,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="24" customHeight="1">
+    <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>38</v>
       </c>
@@ -2093,15 +2178,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" customHeight="1">
+    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="178" customHeight="1">
-      <c r="B16" s="11"/>
-    </row>
-    <row r="18" spans="1:30" ht="24" customHeight="1">
+    <row r="16" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="15" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>52</v>
       </c>
@@ -2109,7 +2196,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:30" ht="24" customHeight="1">
+    <row r="19" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>54</v>
       </c>
@@ -2120,8 +2207,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="24" customHeight="1">
-      <c r="B20" s="11"/>
+    <row r="20" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="AA20" s="6" t="s">
         <v>57</v>
       </c>
@@ -2135,7 +2224,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:30" ht="24" customHeight="1">
+    <row r="22" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>61</v>
       </c>
@@ -2143,7 +2232,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="24" customHeight="1">
+    <row r="23" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>54</v>
       </c>
@@ -2154,8 +2243,10 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:30" ht="24" customHeight="1">
-      <c r="B24" s="11"/>
+    <row r="24" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="AA24" s="6" t="s">
         <v>65</v>
       </c>
@@ -2166,7 +2257,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="24" customHeight="1">
+    <row r="26" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>68</v>
       </c>
@@ -2174,7 +2265,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:30" ht="24" customHeight="1">
+    <row r="27" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>38</v>
       </c>
@@ -2185,15 +2276,17 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="24" customHeight="1">
+    <row r="28" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:30" ht="24" customHeight="1">
-      <c r="B29" s="11"/>
-    </row>
-    <row r="31" spans="1:30" ht="24" customHeight="1">
+    <row r="29" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="11" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>72</v>
       </c>
@@ -2201,7 +2294,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:30" ht="24" customHeight="1">
+    <row r="32" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>38</v>
       </c>
@@ -2212,17 +2305,17 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="24" customHeight="1">
+    <row r="33" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="24" customHeight="1">
+    <row r="34" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="24" customHeight="1">
+    <row r="36" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>77</v>
       </c>
@@ -2230,7 +2323,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="24" customHeight="1">
+    <row r="37" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>38</v>
       </c>
@@ -2241,15 +2334,17 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="24" customHeight="1">
+    <row r="38" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="24" customHeight="1">
-      <c r="B39" s="11"/>
-    </row>
-    <row r="41" spans="1:3" ht="24" customHeight="1">
+    <row r="39" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="11" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>81</v>
       </c>
@@ -2257,7 +2352,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="24" customHeight="1">
+    <row r="42" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>38</v>
       </c>
@@ -2268,10 +2363,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="24" customHeight="1">
-      <c r="B43" s="11"/>
-    </row>
-    <row r="46" spans="1:3" ht="24" customHeight="1">
+    <row r="43" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="11" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>85</v>
       </c>
@@ -2279,12 +2376,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="24" customHeight="1">
+    <row r="47" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:28" ht="24" customHeight="1">
+    <row r="49" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>88</v>
       </c>
@@ -2292,7 +2389,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="24" customHeight="1">
+    <row r="50" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
         <v>54</v>
       </c>
@@ -2303,7 +2400,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="24" customHeight="1">
+    <row r="51" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="11" t="s">
         <v>92</v>
       </c>
@@ -2314,7 +2411,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="24" customHeight="1">
+    <row r="53" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
         <v>95</v>
       </c>
@@ -2322,7 +2419,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="24" customHeight="1">
+    <row r="54" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="14" t="s">
         <v>97</v>
       </c>
@@ -2333,10 +2430,10 @@
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="24" customHeight="1">
+    <row r="55" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="11"/>
     </row>
-    <row r="58" spans="1:28" ht="24" customHeight="1">
+    <row r="58" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="s">
         <v>100</v>
       </c>
@@ -2344,12 +2441,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="24" customHeight="1">
+    <row r="59" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="13" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="1:28" ht="24" customHeight="1">
+    <row r="61" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
         <v>103</v>
       </c>
@@ -2357,7 +2454,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="24" customHeight="1">
+    <row r="62" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
         <v>54</v>
       </c>
@@ -2368,8 +2465,10 @@
         <v>105</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="24" customHeight="1">
-      <c r="B63" s="11"/>
+    <row r="63" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="11" t="s">
+        <v>93</v>
+      </c>
       <c r="AA63" s="6" t="s">
         <v>93</v>
       </c>
@@ -2377,7 +2476,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="24" customHeight="1">
+    <row r="65" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
         <v>106</v>
       </c>
@@ -2385,7 +2484,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="24" customHeight="1">
+    <row r="66" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="14" t="s">
         <v>97</v>
       </c>
@@ -2396,10 +2495,10 @@
         <v>108</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="24" customHeight="1">
+    <row r="67" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="11"/>
     </row>
-    <row r="70" spans="1:28" ht="24" customHeight="1">
+    <row r="70" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="12" t="s">
         <v>109</v>
       </c>
@@ -2407,12 +2506,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="24" customHeight="1">
+    <row r="71" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="73" spans="1:28" ht="24" customHeight="1">
+    <row r="73" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
         <v>112</v>
       </c>
@@ -2420,7 +2519,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="74" spans="1:28" ht="24" customHeight="1">
+    <row r="74" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="14" t="s">
         <v>54</v>
       </c>
@@ -2431,8 +2530,10 @@
         <v>115</v>
       </c>
     </row>
-    <row r="75" spans="1:28" ht="24" customHeight="1">
-      <c r="B75" s="11"/>
+    <row r="75" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="11" t="s">
+        <v>117</v>
+      </c>
       <c r="AA75" s="6" t="s">
         <v>116</v>
       </c>
@@ -2440,7 +2541,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="24" customHeight="1">
+    <row r="77" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
         <v>118</v>
       </c>
@@ -2448,7 +2549,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="24" customHeight="1">
+    <row r="78" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="14" t="s">
         <v>54</v>
       </c>
@@ -2459,8 +2560,10 @@
         <v>121</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="24" customHeight="1">
-      <c r="B79" s="11"/>
+    <row r="79" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B79" s="11" t="s">
+        <v>122</v>
+      </c>
       <c r="AA79" s="6" t="s">
         <v>122</v>
       </c>
@@ -2468,7 +2571,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="81" spans="1:29" ht="24" customHeight="1">
+    <row r="81" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
         <v>123</v>
       </c>
@@ -2476,7 +2579,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="82" spans="1:29" ht="24" customHeight="1">
+    <row r="82" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="14" t="s">
         <v>38</v>
       </c>
@@ -2487,15 +2590,15 @@
         <v>126</v>
       </c>
     </row>
-    <row r="83" spans="1:29" ht="24" customHeight="1">
+    <row r="83" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="84" spans="1:29" ht="178" customHeight="1">
+    <row r="84" spans="1:29" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="11"/>
     </row>
-    <row r="87" spans="1:29" ht="24" customHeight="1">
+    <row r="87" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="12" t="s">
         <v>127</v>
       </c>
@@ -2503,12 +2606,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:29" ht="24" customHeight="1">
+    <row r="88" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B88" s="13" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="90" spans="1:29" ht="24" customHeight="1">
+    <row r="90" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="9" t="s">
         <v>130</v>
       </c>
@@ -2516,7 +2619,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="91" spans="1:29" ht="24" customHeight="1">
+    <row r="91" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="14" t="s">
         <v>54</v>
       </c>
@@ -2527,8 +2630,10 @@
         <v>133</v>
       </c>
     </row>
-    <row r="92" spans="1:29" ht="24" customHeight="1">
-      <c r="B92" s="11"/>
+    <row r="92" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B92" s="11" t="s">
+        <v>134</v>
+      </c>
       <c r="AA92" s="6" t="s">
         <v>134</v>
       </c>
@@ -2539,7 +2644,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="94" spans="1:29" ht="24" customHeight="1">
+    <row r="94" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="9" t="s">
         <v>137</v>
       </c>
@@ -2547,7 +2652,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="95" spans="1:29" ht="24" customHeight="1">
+    <row r="95" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="14" t="s">
         <v>54</v>
       </c>
@@ -2558,8 +2663,10 @@
         <v>140</v>
       </c>
     </row>
-    <row r="96" spans="1:29" ht="24" customHeight="1">
-      <c r="B96" s="11"/>
+    <row r="96" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B96" s="11" t="s">
+        <v>134</v>
+      </c>
       <c r="AA96" s="6" t="s">
         <v>134</v>
       </c>
@@ -2570,7 +2677,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="24" customHeight="1">
+    <row r="98" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="9" t="s">
         <v>142</v>
       </c>
@@ -2578,7 +2685,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="24" customHeight="1">
+    <row r="99" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="14" t="s">
         <v>38</v>
       </c>
@@ -2589,15 +2696,15 @@
         <v>145</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="24" customHeight="1">
+    <row r="100" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="24" customHeight="1">
+    <row r="101" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="11"/>
     </row>
-    <row r="103" spans="1:3" ht="24" customHeight="1">
+    <row r="103" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
         <v>146</v>
       </c>
@@ -2605,7 +2712,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="24" customHeight="1">
+    <row r="104" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="14" t="s">
         <v>38</v>
       </c>
@@ -2616,15 +2723,15 @@
         <v>149</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="24" customHeight="1">
+    <row r="105" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="24" customHeight="1">
+    <row r="106" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B106" s="11"/>
     </row>
-    <row r="109" spans="1:3" ht="24" customHeight="1">
+    <row r="109" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="12" t="s">
         <v>150</v>
       </c>
@@ -2632,12 +2739,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="24" customHeight="1">
+    <row r="110" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="13" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="24" customHeight="1">
+    <row r="112" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="9" t="s">
         <v>153</v>
       </c>
@@ -2645,7 +2752,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="113" spans="1:28" ht="24" customHeight="1">
+    <row r="113" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="14" t="s">
         <v>155</v>
       </c>
@@ -2656,12 +2763,12 @@
         <v>157</v>
       </c>
     </row>
-    <row r="114" spans="1:28" ht="24" customHeight="1">
+    <row r="114" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B114" s="11" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:28" ht="24" customHeight="1">
+    <row r="116" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="9" t="s">
         <v>158</v>
       </c>
@@ -2669,7 +2776,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="117" spans="1:28" ht="24" customHeight="1">
+    <row r="117" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="14" t="s">
         <v>54</v>
       </c>
@@ -2680,7 +2787,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="118" spans="1:28" ht="24" customHeight="1">
+    <row r="118" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B118" s="11" t="s">
         <v>162</v>
       </c>
@@ -2691,7 +2798,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="120" spans="1:28" ht="24" customHeight="1">
+    <row r="120" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="9" t="s">
         <v>164</v>
       </c>
@@ -2699,7 +2806,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="121" spans="1:28" ht="24" customHeight="1">
+    <row r="121" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="14" t="s">
         <v>155</v>
       </c>
@@ -2710,12 +2817,12 @@
         <v>167</v>
       </c>
     </row>
-    <row r="122" spans="1:28" ht="24" customHeight="1">
+    <row r="122" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B122" s="11" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:28" ht="24" customHeight="1">
+    <row r="124" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="9" t="s">
         <v>168</v>
       </c>
@@ -2723,7 +2830,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="125" spans="1:28" ht="24" customHeight="1">
+    <row r="125" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="14" t="s">
         <v>54</v>
       </c>
@@ -2734,7 +2841,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="126" spans="1:28" ht="24" customHeight="1">
+    <row r="126" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B126" s="11" t="s">
         <v>162</v>
       </c>
@@ -2745,7 +2852,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="128" spans="1:28" ht="24" customHeight="1">
+    <row r="128" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="9" t="s">
         <v>172</v>
       </c>
@@ -2753,7 +2860,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="24" customHeight="1">
+    <row r="129" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="14" t="s">
         <v>155</v>
       </c>
@@ -2764,12 +2871,12 @@
         <v>175</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="24" customHeight="1">
+    <row r="130" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B130" s="11" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="24" customHeight="1">
+    <row r="132" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="9" t="s">
         <v>176</v>
       </c>
@@ -2777,7 +2884,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="24" customHeight="1">
+    <row r="133" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="14" t="s">
         <v>38</v>
       </c>
@@ -2788,10 +2895,12 @@
         <v>179</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="24" customHeight="1">
-      <c r="B134" s="11"/>
-    </row>
-    <row r="136" spans="1:3" ht="24" customHeight="1">
+    <row r="134" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B134" s="11" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="9" t="s">
         <v>180</v>
       </c>
@@ -2799,7 +2908,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="24" customHeight="1">
+    <row r="137" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="14" t="s">
         <v>155</v>
       </c>
@@ -2810,12 +2919,12 @@
         <v>183</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="24" customHeight="1">
+    <row r="138" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B138" s="11" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="24" customHeight="1">
+    <row r="140" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="9" t="s">
         <v>184</v>
       </c>
@@ -2823,7 +2932,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="24" customHeight="1">
+    <row r="141" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="14" t="s">
         <v>38</v>
       </c>
@@ -2834,10 +2943,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="24" customHeight="1">
-      <c r="B142" s="11"/>
-    </row>
-    <row r="144" spans="1:3" ht="24" customHeight="1">
+    <row r="142" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B142" s="11" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="9" t="s">
         <v>188</v>
       </c>
@@ -2845,7 +2956,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="24" customHeight="1">
+    <row r="145" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="14" t="s">
         <v>155</v>
       </c>
@@ -2856,12 +2967,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="24" customHeight="1">
+    <row r="146" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B146" s="11" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="24" customHeight="1">
+    <row r="148" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="9" t="s">
         <v>192</v>
       </c>
@@ -2869,7 +2980,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="24" customHeight="1">
+    <row r="149" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="14" t="s">
         <v>38</v>
       </c>
@@ -2880,10 +2991,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="24" customHeight="1">
-      <c r="B150" s="11"/>
-    </row>
-    <row r="152" spans="1:3" ht="24" customHeight="1">
+    <row r="150" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B150" s="11" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="9" t="s">
         <v>196</v>
       </c>
@@ -2891,7 +3004,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="24" customHeight="1">
+    <row r="153" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="14" t="s">
         <v>155</v>
       </c>
@@ -2902,10 +3015,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="24" customHeight="1">
-      <c r="B154" s="11"/>
-    </row>
-    <row r="156" spans="1:3" ht="24" customHeight="1">
+    <row r="154" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B154" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="9" t="s">
         <v>200</v>
       </c>
@@ -2913,7 +3028,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="24" customHeight="1">
+    <row r="157" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="14" t="s">
         <v>38</v>
       </c>
@@ -2924,10 +3039,12 @@
         <v>203</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="24" customHeight="1">
-      <c r="B158" s="11"/>
-    </row>
-    <row r="160" spans="1:3" ht="24" customHeight="1">
+    <row r="158" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B158" s="11" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="9" t="s">
         <v>204</v>
       </c>
@@ -2935,7 +3052,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="24" customHeight="1">
+    <row r="161" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="14" t="s">
         <v>155</v>
       </c>
@@ -2946,10 +3063,12 @@
         <v>207</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="24" customHeight="1">
-      <c r="B162" s="11"/>
-    </row>
-    <row r="164" spans="1:3" ht="24" customHeight="1">
+    <row r="162" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B162" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="9" t="s">
         <v>208</v>
       </c>
@@ -2957,7 +3076,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="24" customHeight="1">
+    <row r="165" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="14" t="s">
         <v>38</v>
       </c>
@@ -2968,10 +3087,12 @@
         <v>211</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="24" customHeight="1">
-      <c r="B166" s="11"/>
-    </row>
-    <row r="168" spans="1:3" ht="24" customHeight="1">
+    <row r="166" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B166" s="11" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="9" t="s">
         <v>212</v>
       </c>
@@ -2979,7 +3100,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="24" customHeight="1">
+    <row r="169" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="14" t="s">
         <v>155</v>
       </c>
@@ -2990,10 +3111,12 @@
         <v>215</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="24" customHeight="1">
-      <c r="B170" s="11"/>
-    </row>
-    <row r="172" spans="1:3" ht="24" customHeight="1">
+    <row r="170" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B170" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="9" t="s">
         <v>216</v>
       </c>
@@ -3001,7 +3124,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="24" customHeight="1">
+    <row r="173" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="14" t="s">
         <v>38</v>
       </c>
@@ -3012,10 +3135,12 @@
         <v>219</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="24" customHeight="1">
-      <c r="B174" s="11"/>
-    </row>
-    <row r="176" spans="1:3" ht="24" customHeight="1">
+    <row r="174" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B174" s="11" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="9" t="s">
         <v>220</v>
       </c>
@@ -3023,7 +3148,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="24" customHeight="1">
+    <row r="177" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="14" t="s">
         <v>155</v>
       </c>
@@ -3034,10 +3159,12 @@
         <v>223</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="24" customHeight="1">
-      <c r="B178" s="11"/>
-    </row>
-    <row r="180" spans="1:3" ht="24" customHeight="1">
+    <row r="178" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B178" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="9" t="s">
         <v>224</v>
       </c>
@@ -3045,7 +3172,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="24" customHeight="1">
+    <row r="181" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="14" t="s">
         <v>38</v>
       </c>
@@ -3056,10 +3183,10 @@
         <v>227</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="24" customHeight="1">
+    <row r="182" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B182" s="11"/>
     </row>
-    <row r="184" spans="1:3" ht="24" customHeight="1">
+    <row r="184" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="9" t="s">
         <v>228</v>
       </c>
@@ -3067,7 +3194,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="24" customHeight="1">
+    <row r="185" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="14" t="s">
         <v>155</v>
       </c>
@@ -3078,10 +3205,12 @@
         <v>231</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="24" customHeight="1">
-      <c r="B186" s="11"/>
-    </row>
-    <row r="188" spans="1:3" ht="24" customHeight="1">
+    <row r="186" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B186" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="9" t="s">
         <v>232</v>
       </c>
@@ -3089,7 +3218,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="24" customHeight="1">
+    <row r="189" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="14" t="s">
         <v>38</v>
       </c>
@@ -3100,10 +3229,10 @@
         <v>235</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="24" customHeight="1">
+    <row r="190" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B190" s="11"/>
     </row>
-    <row r="192" spans="1:3" ht="24" customHeight="1">
+    <row r="192" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="9" t="s">
         <v>236</v>
       </c>
@@ -3111,7 +3240,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="193" spans="1:29" ht="24" customHeight="1">
+    <row r="193" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="14" t="s">
         <v>38</v>
       </c>
@@ -3122,10 +3251,10 @@
         <v>239</v>
       </c>
     </row>
-    <row r="194" spans="1:29" ht="24" customHeight="1">
+    <row r="194" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B194" s="11"/>
     </row>
-    <row r="197" spans="1:29" ht="24" customHeight="1">
+    <row r="197" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="12" t="s">
         <v>240</v>
       </c>
@@ -3133,12 +3262,12 @@
         <v>241</v>
       </c>
     </row>
-    <row r="198" spans="1:29" ht="24" customHeight="1">
+    <row r="198" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B198" s="13" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="200" spans="1:29" ht="24" customHeight="1">
+    <row r="200" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="9" t="s">
         <v>243</v>
       </c>
@@ -3146,7 +3275,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="201" spans="1:29" ht="24" customHeight="1">
+    <row r="201" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="14" t="s">
         <v>54</v>
       </c>
@@ -3157,8 +3286,10 @@
         <v>245</v>
       </c>
     </row>
-    <row r="202" spans="1:29" ht="24" customHeight="1">
-      <c r="B202" s="11"/>
+    <row r="202" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B202" s="11" t="s">
+        <v>163</v>
+      </c>
       <c r="AA202" s="6" t="s">
         <v>163</v>
       </c>
@@ -3166,7 +3297,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="204" spans="1:29" ht="24" customHeight="1">
+    <row r="204" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="9" t="s">
         <v>247</v>
       </c>
@@ -3174,7 +3305,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="205" spans="1:29" ht="24" customHeight="1">
+    <row r="205" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="14" t="s">
         <v>54</v>
       </c>
@@ -3185,7 +3316,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="206" spans="1:29" ht="24" customHeight="1">
+    <row r="206" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B206" s="11" t="s">
         <v>251</v>
       </c>
@@ -3199,7 +3330,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="208" spans="1:29" ht="24" customHeight="1">
+    <row r="208" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="9" t="s">
         <v>253</v>
       </c>
@@ -3207,7 +3338,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="24" customHeight="1">
+    <row r="209" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="14" t="s">
         <v>38</v>
       </c>
@@ -3218,15 +3349,15 @@
         <v>256</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="24" customHeight="1">
+    <row r="210" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B210" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="24" customHeight="1">
+    <row r="211" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B211" s="11"/>
     </row>
-    <row r="214" spans="1:3" ht="24" customHeight="1">
+    <row r="214" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="12" t="s">
         <v>257</v>
       </c>
@@ -3234,12 +3365,12 @@
         <v>258</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="24" customHeight="1">
+    <row r="215" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B215" s="13" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="24" customHeight="1">
+    <row r="217" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="9" t="s">
         <v>260</v>
       </c>
@@ -3247,7 +3378,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="24" customHeight="1">
+    <row r="218" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="14" t="s">
         <v>38</v>
       </c>
@@ -3258,15 +3389,17 @@
         <v>263</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="24" customHeight="1">
+    <row r="219" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B219" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="178" customHeight="1">
-      <c r="B220" s="11"/>
-    </row>
-    <row r="222" spans="1:3" ht="24" customHeight="1">
+    <row r="220" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B220" s="11" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="9" t="s">
         <v>264</v>
       </c>
@@ -3274,7 +3407,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="24" customHeight="1">
+    <row r="223" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="14" t="s">
         <v>38</v>
       </c>
@@ -3285,15 +3418,17 @@
         <v>267</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="24" customHeight="1">
+    <row r="224" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B224" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="24" customHeight="1">
-      <c r="B225" s="11"/>
-    </row>
-    <row r="227" spans="1:3" ht="24" customHeight="1">
+    <row r="225" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B225" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="9" t="s">
         <v>268</v>
       </c>
@@ -3301,7 +3436,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="228" spans="1:3" ht="24" customHeight="1">
+    <row r="228" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="14" t="s">
         <v>38</v>
       </c>
@@ -3312,15 +3447,15 @@
         <v>271</v>
       </c>
     </row>
-    <row r="229" spans="1:3" ht="24" customHeight="1">
+    <row r="229" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B229" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="230" spans="1:3" ht="24" customHeight="1">
+    <row r="230" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B230" s="11"/>
     </row>
-    <row r="232" spans="1:3" ht="24" customHeight="1">
+    <row r="232" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="9" t="s">
         <v>272</v>
       </c>
@@ -3328,7 +3463,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="24" customHeight="1">
+    <row r="233" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="14" t="s">
         <v>38</v>
       </c>
@@ -3339,87 +3474,30 @@
         <v>275</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="24" customHeight="1">
+    <row r="234" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B234" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="235" spans="1:3" ht="24" customHeight="1">
+    <row r="235" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B235" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="24">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>AA20:AD20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24 B206 B96 B92" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>AA24:AC24</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51 B202 B126 B118 B79 B75 B63" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>AA51:AB51</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55 B67" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63">
-      <formula1>AA63:AB63</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B67">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75">
-      <formula1>AA75:AB75</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79">
-      <formula1>AA79:AB79</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B92">
-      <formula1>AA92:AC92</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B96">
-      <formula1>AA96:AC96</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B114">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B114 B186 B178 B170 B162 B154 B146 B138 B130 B122" xr:uid="{00000000-0002-0000-0200-00000A000000}">
       <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B118">
-      <formula1>AA118:AB118</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B122">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B126">
-      <formula1>AA126:AB126</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B130">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B138">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B146">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B154">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B162">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B170">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B178">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B186">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B202">
-      <formula1>AA202:AB202</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B206">
-      <formula1>AA206:AC206</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3427,20 +3505,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD128"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AE131"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" customHeight="1">
+    <row r="1" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>276</v>
       </c>
@@ -3448,12 +3528,12 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" customHeight="1">
+    <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>279</v>
       </c>
@@ -3461,7 +3541,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" customHeight="1">
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>38</v>
       </c>
@@ -3472,10 +3552,12 @@
         <v>281</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
-    </row>
-    <row r="8" spans="1:3" ht="24" customHeight="1">
+    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>282</v>
       </c>
@@ -3483,7 +3565,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24" customHeight="1">
+    <row r="9" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>38</v>
       </c>
@@ -3494,15 +3576,17 @@
         <v>284</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24" customHeight="1">
+    <row r="10" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
-    </row>
-    <row r="13" spans="1:3" ht="24" customHeight="1">
+    <row r="11" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>285</v>
       </c>
@@ -3510,7 +3594,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="24" customHeight="1">
+    <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>155</v>
       </c>
@@ -3521,12 +3605,12 @@
         <v>288</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" customHeight="1">
+    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="24" customHeight="1">
+    <row r="17" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>289</v>
       </c>
@@ -3534,7 +3618,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="24" customHeight="1">
+    <row r="18" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>54</v>
       </c>
@@ -3545,13 +3629,15 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="24" customHeight="1">
+    <row r="19" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="24" customHeight="1">
-      <c r="B20" s="11"/>
+    <row r="20" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="11" t="s">
+        <v>293</v>
+      </c>
       <c r="AA20" s="6" t="s">
         <v>293</v>
       </c>
@@ -3568,761 +3654,788 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="24" customHeight="1">
-      <c r="A22" s="9" t="s">
+    <row r="21" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="AA21" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="AB21" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="AC21" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="AD21" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="AE21" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="AA22" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="AB22" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="AC22" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="AD22" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="AE22" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="AA23" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="AB23" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="AC23" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="AD23" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="AE23" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B25" s="9" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="24" customHeight="1">
-      <c r="A23" s="14" t="s">
+    <row r="26" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B26" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C26" s="10" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="24" customHeight="1">
-      <c r="B24" s="10" t="s">
+    <row r="27" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="24" customHeight="1">
-      <c r="B25" s="11"/>
-      <c r="AA25" s="6" t="s">
+    <row r="28" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="AB25" s="6" t="s">
+      <c r="AA28" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="AB28" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="AC25" s="6" t="s">
+      <c r="AC28" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="24" customHeight="1">
-      <c r="A27" s="9" t="s">
+    <row r="30" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B30" s="9" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="24" customHeight="1">
-      <c r="A28" s="14" t="s">
+    <row r="31" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B31" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C31" s="10" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="24" customHeight="1">
-      <c r="B29" s="10" t="s">
+    <row r="32" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="24" customHeight="1">
-      <c r="B30" s="11"/>
-      <c r="AA30" s="6" t="s">
+    <row r="33" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="AA33" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="AB30" s="6" t="s">
+      <c r="AB33" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="AC30" s="6" t="s">
+      <c r="AC33" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="24" customHeight="1">
-      <c r="A33" s="12" t="s">
+    <row r="36" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
         <v>309</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B36" s="12" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="24" customHeight="1">
-      <c r="B34" s="13" t="s">
+    <row r="37" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="13" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="24" customHeight="1">
-      <c r="A36" s="9" t="s">
+    <row r="39" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="24" customHeight="1">
-      <c r="A37" s="14" t="s">
+    <row r="40" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B40" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C40" s="10" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="24" customHeight="1">
-      <c r="B38" s="11"/>
-    </row>
-    <row r="40" spans="1:3" ht="24" customHeight="1">
-      <c r="A40" s="9" t="s">
+    <row r="41" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="11"/>
+    </row>
+    <row r="43" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B43" s="9" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="24" customHeight="1">
-      <c r="A41" s="14" t="s">
+    <row r="44" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B44" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C44" s="10" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="24" customHeight="1">
-      <c r="B42" s="11"/>
-    </row>
-    <row r="45" spans="1:3" ht="24" customHeight="1">
-      <c r="A45" s="12" t="s">
+    <row r="45" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="11"/>
+    </row>
+    <row r="48" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="12" t="s">
         <v>320</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B48" s="12" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="24" customHeight="1">
-      <c r="B46" s="13" t="s">
+    <row r="49" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="13" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="24" customHeight="1">
-      <c r="A48" s="9" t="s">
+    <row r="51" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="9" t="s">
         <v>323</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B51" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="49" spans="1:31" ht="24" customHeight="1">
-      <c r="A49" s="14" t="s">
+    <row r="52" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B52" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C52" s="10" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="50" spans="1:31" ht="24" customHeight="1">
-      <c r="B50" s="11" t="s">
+    <row r="53" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="AA50" s="6" t="s">
+      <c r="AA53" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="AB50" s="6" t="s">
+      <c r="AB53" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="AC50" s="6" t="s">
+      <c r="AC53" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="AD50" s="6" t="s">
+      <c r="AD53" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="AE50" s="6" t="s">
+      <c r="AE53" s="6" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="52" spans="1:31" ht="24" customHeight="1">
-      <c r="A52" s="9" t="s">
+    <row r="55" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B55" s="9" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="53" spans="1:31" ht="24" customHeight="1">
-      <c r="A53" s="14" t="s">
+    <row r="56" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B56" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C56" s="10" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="54" spans="1:31" ht="24" customHeight="1">
-      <c r="B54" s="10" t="s">
+    <row r="57" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:31" ht="24" customHeight="1">
-      <c r="B55" s="11"/>
-      <c r="AA55" s="6" t="s">
+    <row r="58" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="11"/>
+      <c r="AA58" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="AB55" s="6" t="s">
+      <c r="AB58" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="AC55" s="6" t="s">
+      <c r="AC58" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="AD55" s="6" t="s">
+      <c r="AD58" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:31" ht="24" customHeight="1">
-      <c r="A57" s="9" t="s">
+    <row r="60" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="9" t="s">
         <v>338</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B60" s="9" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="58" spans="1:31" ht="24" customHeight="1">
-      <c r="A58" s="14" t="s">
+    <row r="61" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B61" s="10" t="s">
         <v>340</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C61" s="10" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="59" spans="1:31" ht="24" customHeight="1">
-      <c r="B59" s="10" t="s">
+    <row r="62" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:31" ht="24" customHeight="1">
-      <c r="B60" s="11"/>
-      <c r="AA60" s="6" t="s">
+    <row r="63" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="11"/>
+      <c r="AA63" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="AB60" s="6" t="s">
+      <c r="AB63" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="AC60" s="6" t="s">
+      <c r="AC63" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="AD60" s="6" t="s">
+      <c r="AD63" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:31" ht="24" customHeight="1">
-      <c r="A63" s="12" t="s">
+    <row r="66" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="B63" s="12" t="s">
+      <c r="B66" s="12" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="64" spans="1:31" ht="24" customHeight="1">
-      <c r="B64" s="13" t="s">
+    <row r="67" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="13" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="66" spans="1:30" ht="24" customHeight="1">
-      <c r="A66" s="9" t="s">
+    <row r="69" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B69" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="67" spans="1:30" ht="24" customHeight="1">
-      <c r="A67" s="14" t="s">
+    <row r="70" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B70" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C70" s="10" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="68" spans="1:30" ht="24" customHeight="1">
-      <c r="B68" s="11" t="s">
+    <row r="71" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="AA68" s="6" t="s">
+      <c r="AA71" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="AB68" s="6" t="s">
+      <c r="AB71" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="AC68" s="6" t="s">
+      <c r="AC71" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="AD68" s="6" t="s">
+      <c r="AD71" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:30" ht="24" customHeight="1">
-      <c r="A70" s="9" t="s">
+    <row r="73" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B73" s="9" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="71" spans="1:30" ht="24" customHeight="1">
-      <c r="A71" s="14" t="s">
+    <row r="74" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B71" s="10" t="s">
+      <c r="B74" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="C71" s="10" t="s">
+      <c r="C74" s="10" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="72" spans="1:30" ht="24" customHeight="1">
-      <c r="B72" s="10" t="s">
+    <row r="75" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:30" ht="24" customHeight="1">
-      <c r="B73" s="11"/>
-      <c r="AA73" s="6" t="s">
+    <row r="76" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="11"/>
+      <c r="AA76" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="AB73" s="6" t="s">
+      <c r="AB76" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="AC73" s="6" t="s">
+      <c r="AC76" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:30" ht="24" customHeight="1">
-      <c r="A76" s="12" t="s">
+    <row r="79" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="B76" s="12" t="s">
+      <c r="B79" s="12" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="77" spans="1:30" ht="24" customHeight="1">
-      <c r="B77" s="13" t="s">
+    <row r="80" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B80" s="13" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="79" spans="1:30" ht="24" customHeight="1">
-      <c r="A79" s="9" t="s">
+    <row r="82" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="B79" s="9" t="s">
+      <c r="B82" s="9" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="80" spans="1:30" ht="24" customHeight="1">
-      <c r="A80" s="14" t="s">
+    <row r="83" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="B80" s="10" t="s">
+      <c r="B83" s="10" t="s">
         <v>362</v>
       </c>
-      <c r="C80" s="10" t="s">
+      <c r="C83" s="10" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="81" spans="1:31" ht="24" customHeight="1">
-      <c r="B81" s="11"/>
-    </row>
-    <row r="83" spans="1:31" ht="24" customHeight="1">
-      <c r="A83" s="9" t="s">
+    <row r="84" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B84" s="11"/>
+    </row>
+    <row r="86" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="B83" s="9" t="s">
+      <c r="B86" s="9" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="84" spans="1:31" ht="24" customHeight="1">
-      <c r="A84" s="14" t="s">
+    <row r="87" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B84" s="10" t="s">
+      <c r="B87" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="C84" s="10" t="s">
+      <c r="C87" s="10" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="85" spans="1:31" ht="24" customHeight="1">
-      <c r="B85" s="11" t="s">
+    <row r="88" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B88" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="AA85" s="6" t="s">
+      <c r="AA88" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="AB85" s="6" t="s">
+      <c r="AB88" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="AC85" s="6" t="s">
+      <c r="AC88" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="AD85" s="6" t="s">
+      <c r="AD88" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="AE85" s="6" t="s">
+      <c r="AE88" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="88" spans="1:31" ht="24" customHeight="1">
-      <c r="A88" s="12" t="s">
+    <row r="91" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="12" t="s">
         <v>372</v>
       </c>
-      <c r="B88" s="12" t="s">
+      <c r="B91" s="12" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="89" spans="1:31" ht="24" customHeight="1">
-      <c r="B89" s="13" t="s">
+    <row r="92" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B92" s="13" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="91" spans="1:31" ht="24" customHeight="1">
-      <c r="A91" s="9" t="s">
+    <row r="94" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="B91" s="9" t="s">
+      <c r="B94" s="9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:31" ht="24" customHeight="1">
-      <c r="A92" s="14" t="s">
+    <row r="95" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B92" s="10" t="s">
+      <c r="B95" s="10" t="s">
         <v>376</v>
       </c>
-      <c r="C92" s="10" t="s">
+      <c r="C95" s="10" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="93" spans="1:31" ht="24" customHeight="1">
-      <c r="B93" s="10" t="s">
+    <row r="96" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B96" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:31" ht="24" customHeight="1">
-      <c r="B94" s="11" t="s">
+    <row r="97" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B97" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="AA94" s="6" t="s">
+      <c r="AA97" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="AB94" s="6" t="s">
+      <c r="AB97" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="AC94" s="6" t="s">
+      <c r="AC97" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="AD94" s="6" t="s">
+      <c r="AD97" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="AE94" s="6" t="s">
+      <c r="AE97" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:31" ht="24" customHeight="1">
-      <c r="A96" s="9" t="s">
+    <row r="99" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="B96" s="9" t="s">
+      <c r="B99" s="9" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="97" spans="1:31" ht="24" customHeight="1">
-      <c r="A97" s="14" t="s">
+    <row r="100" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B97" s="10" t="s">
+      <c r="B100" s="10" t="s">
         <v>384</v>
       </c>
-      <c r="C97" s="10" t="s">
+      <c r="C100" s="10" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="98" spans="1:31" ht="24" customHeight="1">
-      <c r="B98" s="10" t="s">
+    <row r="101" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B101" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:31" ht="24" customHeight="1">
-      <c r="B99" s="11"/>
-      <c r="AA99" s="6" t="s">
+    <row r="102" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B102" s="11"/>
+      <c r="AA102" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="AB99" s="6" t="s">
+      <c r="AB102" s="6" t="s">
         <v>387</v>
       </c>
-      <c r="AC99" s="6" t="s">
+      <c r="AC102" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="AD99" s="6" t="s">
+      <c r="AD102" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="AE99" s="6" t="s">
+      <c r="AE102" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="101" spans="1:31" ht="24" customHeight="1">
-      <c r="A101" s="9" t="s">
+    <row r="104" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="B101" s="9" t="s">
+      <c r="B104" s="9" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="102" spans="1:31" ht="24" customHeight="1">
-      <c r="A102" s="14" t="s">
+    <row r="105" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B102" s="10" t="s">
+      <c r="B105" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="C102" s="10" t="s">
+      <c r="C105" s="10" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="103" spans="1:31" ht="24" customHeight="1">
-      <c r="B103" s="11"/>
-      <c r="AA103" s="6" t="s">
+    <row r="106" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B106" s="11"/>
+      <c r="AA106" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="AB103" s="6" t="s">
+      <c r="AB106" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="AC103" s="6" t="s">
+      <c r="AC106" s="6" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="105" spans="1:31" ht="24" customHeight="1">
-      <c r="A105" s="9" t="s">
+    <row r="108" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="B105" s="9" t="s">
+      <c r="B108" s="9" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="106" spans="1:31" ht="24" customHeight="1">
-      <c r="A106" s="14" t="s">
+    <row r="109" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B106" s="10" t="s">
+      <c r="B109" s="10" t="s">
         <v>399</v>
       </c>
-      <c r="C106" s="10" t="s">
+      <c r="C109" s="10" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="107" spans="1:31" ht="24" customHeight="1">
-      <c r="B107" s="11"/>
-    </row>
-    <row r="109" spans="1:31" ht="24" customHeight="1">
-      <c r="A109" s="9" t="s">
+    <row r="110" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B110" s="11"/>
+    </row>
+    <row r="112" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B109" s="9" t="s">
+      <c r="B112" s="9" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="110" spans="1:31" ht="24" customHeight="1">
-      <c r="A110" s="14" t="s">
+    <row r="113" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B110" s="10" t="s">
+      <c r="B113" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="C110" s="10" t="s">
+      <c r="C113" s="10" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="111" spans="1:31" ht="24" customHeight="1">
-      <c r="B111" s="11"/>
-      <c r="AA111" s="6" t="s">
+    <row r="114" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B114" s="11"/>
+      <c r="AA114" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="AB111" s="6" t="s">
+      <c r="AB114" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="AC111" s="6" t="s">
+      <c r="AC114" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="AD111" s="6" t="s">
+      <c r="AD114" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="114" spans="1:28" ht="24" customHeight="1">
-      <c r="A114" s="12" t="s">
+    <row r="117" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="12" t="s">
         <v>408</v>
       </c>
-      <c r="B114" s="12" t="s">
+      <c r="B117" s="12" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="115" spans="1:28" ht="24" customHeight="1">
-      <c r="B115" s="13" t="s">
+    <row r="118" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B118" s="13" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="117" spans="1:28" ht="24" customHeight="1">
-      <c r="A117" s="9" t="s">
+    <row r="120" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="B117" s="9" t="s">
+      <c r="B120" s="9" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="118" spans="1:28" ht="24" customHeight="1">
-      <c r="A118" s="14" t="s">
+    <row r="121" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B118" s="10" t="s">
+      <c r="B121" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="C118" s="10" t="s">
+      <c r="C121" s="10" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="119" spans="1:28" ht="24" customHeight="1">
-      <c r="B119" s="10" t="s">
+    <row r="122" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B122" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="120" spans="1:28" ht="24" customHeight="1">
-      <c r="B120" s="11"/>
-      <c r="AA120" s="6" t="s">
+    <row r="123" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B123" s="11"/>
+      <c r="AA123" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="AB120" s="6" t="s">
+      <c r="AB123" s="6" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="122" spans="1:28" ht="24" customHeight="1">
-      <c r="A122" s="9" t="s">
+    <row r="125" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="B122" s="9" t="s">
+      <c r="B125" s="9" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="123" spans="1:28" ht="24" customHeight="1">
-      <c r="A123" s="14" t="s">
+    <row r="126" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="B123" s="10" t="s">
+      <c r="B126" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="C123" s="10" t="s">
+      <c r="C126" s="10" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="124" spans="1:28" ht="24" customHeight="1">
-      <c r="B124" s="11"/>
-    </row>
-    <row r="126" spans="1:28" ht="24" customHeight="1">
-      <c r="A126" s="9" t="s">
+    <row r="127" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B127" s="11"/>
+    </row>
+    <row r="129" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B126" s="9" t="s">
+      <c r="B129" s="9" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="127" spans="1:28" ht="24" customHeight="1">
-      <c r="A127" s="14" t="s">
+    <row r="130" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B127" s="10" t="s">
+      <c r="B130" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="C127" s="10" t="s">
+      <c r="C130" s="10" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="128" spans="1:28" ht="24" customHeight="1">
-      <c r="B128" s="11"/>
-      <c r="AA128" s="6" t="s">
+    <row r="131" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B131" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="AB128" s="6" t="s">
+      <c r="AA131" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="AB131" s="6" t="s">
         <v>425</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="18">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15 B127 B84" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B53 B102 B97 B88 B20:B23" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>AA20:AE20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25">
-      <formula1>AA25:AC25</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28 B106 B76 B33" xr:uid="{00000000-0002-0000-0300-000002000000}">
+      <formula1>AA28:AC28</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30">
-      <formula1>AA30:AC30</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B58 B114 B71 B63" xr:uid="{00000000-0002-0000-0300-000005000000}">
+      <formula1>AA58:AD58</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B50">
-      <formula1>AA50:AE50</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55">
-      <formula1>AA55:AD55</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60">
-      <formula1>AA60:AD60</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B68">
-      <formula1>AA68:AD68</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B73">
-      <formula1>AA73:AC73</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B81">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B85">
-      <formula1>AA85:AE85</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B94">
-      <formula1>AA94:AE94</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B99">
-      <formula1>AA99:AE99</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B103">
-      <formula1>AA103:AC103</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B111">
-      <formula1>AA111:AD111</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B120">
-      <formula1>AA120:AB120</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B124">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B128">
-      <formula1>AA128:AB128</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B123 B131" xr:uid="{00000000-0002-0000-0300-00000F000000}">
+      <formula1>AA123:AB123</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>